<commit_message>
AITATR3-150 & AITATR3-151 Perubahan parsing pada custom keyword
</commit_message>
<xml_diff>
--- a/Rule/InsAddCvgRule.xlsx
+++ b/Rule/InsAddCvgRule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="MainCvg" sheetId="3" r:id="rId1"/>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2775,7 +2775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q236"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix mainrate Insurance not eq click random object + fixrule
</commit_message>
<xml_diff>
--- a/Rule/InsAddCvgRule.xlsx
+++ b/Rule/InsAddCvgRule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="MainCvg" sheetId="3" r:id="rId1"/>
@@ -583,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView topLeftCell="C43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
@@ -2775,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H154" sqref="H154"/>
+    <sheetView topLeftCell="C175" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F229" sqref="F229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>